<commit_message>
Changed final format from csv to tsv to prevent any changes and problems while exchanging databases from a person to another. Other changes : corrected error from the meteo files since some errors were not corrected when the implementation of column content verification was done.
</commit_message>
<xml_diff>
--- a/data/raw/comptages_terrain/meteo/us_med_pnmcca_observatoire_comptage_terrain_meteo_2020-07-20.xlsx
+++ b/data/raw/comptages_terrain/meteo/us_med_pnmcca_observatoire_comptage_terrain_meteo_2020-07-20.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="12180"/>
+    <workbookView windowWidth="27945" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="Meteo" sheetId="3" r:id="rId1"/>
@@ -104,7 +104,7 @@
     <t>Basé sur Lotu 9h</t>
   </si>
   <si>
-    <t>Petit Lotu</t>
+    <t>Mezzanu</t>
   </si>
   <si>
     <t>Basé sur Petit Lotu 9h</t>
@@ -1237,7 +1237,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A1" sqref="A1:K17"/>
+      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>

</xml_diff>